<commit_message>
Update results folder with survey results
</commit_message>
<xml_diff>
--- a/pre-post_experiment/results/PrimaryResults_prepost.xlsx
+++ b/pre-post_experiment/results/PrimaryResults_prepost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhaleh\PhD_Projects\Effects_of_Training_Non-Musicians_in_Beat_Perception_on_Timing_Across_Three_Modalitie\pre-post_experiment\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B1B2BE-206D-4A9B-AC2B-A097B07CFA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424FCB32-7807-41CA-9FFA-F8979A967DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19750" yWindow="-11990" windowWidth="19550" windowHeight="18510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30260" yWindow="-13780" windowWidth="29660" windowHeight="20960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1220,13 +1220,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU43" sqref="AU43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">

</xml_diff>